<commit_message>
Completing Milestone 1 and working on initial setup
</commit_message>
<xml_diff>
--- a/documentation/AssetList.xlsx
+++ b/documentation/AssetList.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\InteractiveGamesAndAudio\igme-671-final-project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D814180-496E-470B-9480-84FC6D9DED24}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1B7D5C-FC79-4241-94FF-8CDDF4EE9395}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="77">
   <si>
     <t>Description</t>
   </si>
@@ -37,13 +37,232 @@
   </si>
   <si>
     <t>Event Name</t>
+  </si>
+  <si>
+    <t>Fireball</t>
+  </si>
+  <si>
+    <t>SoulfirePickup</t>
+  </si>
+  <si>
+    <t>HellfirePickup</t>
+  </si>
+  <si>
+    <t>SoulfireAmbiance</t>
+  </si>
+  <si>
+    <t>HellfireAmbiance</t>
+  </si>
+  <si>
+    <t>TutorialDialog</t>
+  </si>
+  <si>
+    <t>ClickButton</t>
+  </si>
+  <si>
+    <t>HitPauseKey</t>
+  </si>
+  <si>
+    <t>ClickInventoryItem</t>
+  </si>
+  <si>
+    <t>ExitGame</t>
+  </si>
+  <si>
+    <t>SpookyMusic</t>
+  </si>
+  <si>
+    <t>BossMusic</t>
+  </si>
+  <si>
+    <t>LowHealthMusic</t>
+  </si>
+  <si>
+    <t>MenuMusic</t>
+  </si>
+  <si>
+    <t>Ambiance</t>
+  </si>
+  <si>
+    <t>Sound Effect</t>
+  </si>
+  <si>
+    <t>Dialog</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>Interface</t>
+  </si>
+  <si>
+    <t>PlayerAmbiance</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Incomplete</t>
+  </si>
+  <si>
+    <t>Fireball Fire, Fireball Charge</t>
+  </si>
+  <si>
+    <t>PlayerHit</t>
+  </si>
+  <si>
+    <t>EnemyHit</t>
+  </si>
+  <si>
+    <t>Melee Attack Vampire, Melee Attack Thrall, Melee Attack Hellhound</t>
+  </si>
+  <si>
+    <t>EnemyMeleeAttack</t>
+  </si>
+  <si>
+    <t>Player Hit By Fireball, Player Hit By Melee</t>
+  </si>
+  <si>
+    <t>Vampire Hit, Thrall Hit, Hellhound Hit</t>
+  </si>
+  <si>
+    <t>Soulfire Pickup</t>
+  </si>
+  <si>
+    <t>Hellfire Pickup</t>
+  </si>
+  <si>
+    <t>Soulfire Ambiance</t>
+  </si>
+  <si>
+    <t>Hellfire Ambiance</t>
+  </si>
+  <si>
+    <t>Dialog for each statement</t>
+  </si>
+  <si>
+    <t>Click Button</t>
+  </si>
+  <si>
+    <t>Hit Pause Key</t>
+  </si>
+  <si>
+    <t>Click Inventory Item</t>
+  </si>
+  <si>
+    <t>Exit Game</t>
+  </si>
+  <si>
+    <t>Spooky Music</t>
+  </si>
+  <si>
+    <t>Boss Music</t>
+  </si>
+  <si>
+    <t>Low Health Music</t>
+  </si>
+  <si>
+    <t>Menu Music</t>
+  </si>
+  <si>
+    <t>EnemyAmbiance</t>
+  </si>
+  <si>
+    <t>Vampire Ambiance, Thrall Ambiance, Hellhound Ambiance</t>
+  </si>
+  <si>
+    <t>Player Ambiance</t>
+  </si>
+  <si>
+    <t>A sound for when the player is shooting a fireball from their staff. Will include a looping charge sound followed by sound for the fireball shooting.</t>
+  </si>
+  <si>
+    <t>An event for the enemies attacking. Will include sounds that play based on a paramater indicating what type of enemy it is.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An event indicating that the player has been hit by either an enemy melee attack or a spell attack. These will likely be different sounds indicated by a parameter. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">An event indicating whether an enemy has been hit. Will include different sounds for each enemy. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">An event indicating that the soulfire pickup has been obtained. </t>
+  </si>
+  <si>
+    <t>An event indicating that the hellfire pickup has been obtained.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An event that plays as long as the player owns the soulfire item. </t>
+  </si>
+  <si>
+    <t>An event that plays as long as the player owns the hellfire item.</t>
+  </si>
+  <si>
+    <t>Dialog for the tutorial. Will include more than 1 sound file. There will be 1 sound item for each dialog "block".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An interface event for clicking a button. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">An interface event for hitting the pause key on the keyboard. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">An interface event for clicking an item in your inventory. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">An interface event for clicking exit game or the escape key, indicating that the game is closing. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spooky general music that plays throughout the game. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Music that plays in the boss rooms. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Music that plays when the player is at low health. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Music that plays in the menus. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ambiance for the enemies. Will include ambiance for each different type of enemy. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ambiance for the player such as footsteps and breathing. </t>
+  </si>
+  <si>
+    <t>FireballHit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An event indicating that a fireball has hit something. </t>
+  </si>
+  <si>
+    <t>Fireball Hit Entity, Fireball Hit Object</t>
+  </si>
+  <si>
+    <t>HealingTileAmbiance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ambiance for the healing tiles. </t>
+  </si>
+  <si>
+    <t>Healing Tile Ambiance</t>
+  </si>
+  <si>
+    <t>PlayerHealing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charging sound effect for while the player is recovering health while standing on the healing tile. </t>
+  </si>
+  <si>
+    <t>Player Healing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,8 +278,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -73,8 +300,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -106,11 +339,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -118,6 +377,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,21 +661,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -424,6 +688,383 @@
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on creating remaining assets and events.
</commit_message>
<xml_diff>
--- a/documentation/AssetList.xlsx
+++ b/documentation/AssetList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\InteractiveGamesAndAudio\igme-671-final-project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BB62CB-4210-4875-9CE8-CB72FCC1210E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E4901B-64E2-4B87-A522-3D63ABA7B2B5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="95">
   <si>
     <t>Description</t>
   </si>
@@ -69,9 +69,6 @@
     <t>BossMusic</t>
   </si>
   <si>
-    <t>LowHealthMusic</t>
-  </si>
-  <si>
     <t>MenuMusic</t>
   </si>
   <si>
@@ -135,9 +132,6 @@
     <t>Boss Music</t>
   </si>
   <si>
-    <t>Low Health Music</t>
-  </si>
-  <si>
     <t>Menu Music</t>
   </si>
   <si>
@@ -189,9 +183,6 @@
     <t xml:space="preserve">Music that plays in the boss rooms. </t>
   </si>
   <si>
-    <t xml:space="preserve">Music that plays when the player is at low health. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Music that plays in the menus. </t>
   </si>
   <si>
@@ -297,12 +288,6 @@
     <t xml:space="preserve">Not sure what sound I want to do for this exactly yet. </t>
   </si>
   <si>
-    <t>This is going to take some time and recording, but is only for the tutorial so not super critical.</t>
-  </si>
-  <si>
-    <t>Not sure where I'm getting music/what I need to do to it or how to do it</t>
-  </si>
-  <si>
     <t xml:space="preserve">Probably footsteps and some heavy breathing. Will probbaly need to have a setting for standing in place as well. </t>
   </si>
   <si>
@@ -322,6 +307,9 @@
   </si>
   <si>
     <t>Only needed for main menu and other scenes with images of the pc</t>
+  </si>
+  <si>
+    <t>May need to re-record with stereo eventually. Didn't realize it was only recording mono till it was already in FMOD and I'm not sure how much I like it</t>
   </si>
 </sst>
 </file>
@@ -720,10 +708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,16 +739,16 @@
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -768,166 +756,166 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -935,22 +923,22 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -958,22 +946,22 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -981,25 +969,25 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1007,25 +995,25 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H12" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1033,25 +1021,25 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H13" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1059,22 +1047,22 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1082,71 +1070,71 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H17" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1154,25 +1142,22 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>22</v>
+        <v>33</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H18" t="s">
-        <v>91</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1180,25 +1165,22 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H19" t="s">
-        <v>91</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1206,181 +1188,152 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>36</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H20" t="s">
-        <v>91</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" t="s">
         <v>15</v>
       </c>
-      <c r="B21" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" t="s">
-        <v>19</v>
-      </c>
       <c r="D21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>22</v>
+        <v>64</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H21" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D22" t="s">
-        <v>67</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>22</v>
+        <v>37</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H22" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D23" t="s">
-        <v>39</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>22</v>
+        <v>59</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="H23" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="C24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D24" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="H24" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="B25" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="C25" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D25" t="s">
-        <v>83</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>22</v>
+        <v>92</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H25" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>95</v>
-      </c>
-      <c r="B26" t="s">
-        <v>96</v>
-      </c>
-      <c r="C26" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" t="s">
-        <v>97</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H26" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on implementing assets
</commit_message>
<xml_diff>
--- a/documentation/AssetList.xlsx
+++ b/documentation/AssetList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\InteractiveGamesAndAudio\igme-671-final-project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E4901B-64E2-4B87-A522-3D63ABA7B2B5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7502C0-C668-4161-AFF3-B6D15F0C6DBB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="96">
   <si>
     <t>Description</t>
   </si>
@@ -135,9 +135,6 @@
     <t>Menu Music</t>
   </si>
   <si>
-    <t>EnemyAmbiance</t>
-  </si>
-  <si>
     <t>Player Ambiance</t>
   </si>
   <si>
@@ -219,9 +216,6 @@
     <t>Melee Attack Vampire, Melee Attack Hellhound</t>
   </si>
   <si>
-    <t>Vampire Ambiance, Hellhound Ambiance</t>
-  </si>
-  <si>
     <t>Player Hit</t>
   </si>
   <si>
@@ -282,18 +276,9 @@
     <t>Not sure I like the vampire attack sound.</t>
   </si>
   <si>
-    <t>Only needed for final level</t>
-  </si>
-  <si>
     <t xml:space="preserve">Not sure what sound I want to do for this exactly yet. </t>
   </si>
   <si>
-    <t xml:space="preserve">Probably footsteps and some heavy breathing. Will probbaly need to have a setting for standing in place as well. </t>
-  </si>
-  <si>
-    <t>Probably footsteps and some other distinguishing feature. Will need a setting for standing in place. Will likely be a 3D Event</t>
-  </si>
-  <si>
     <t xml:space="preserve">Changed to 3D event. Currently always playing if there is a healing tile in the level, but I'm not sure why. </t>
   </si>
   <si>
@@ -306,10 +291,28 @@
     <t>Fire Crackling</t>
   </si>
   <si>
-    <t>Only needed for main menu and other scenes with images of the pc</t>
-  </si>
-  <si>
     <t>May need to re-record with stereo eventually. Didn't realize it was only recording mono till it was already in FMOD and I'm not sure how much I like it</t>
+  </si>
+  <si>
+    <t>Is playing, but volume needs some attention in mixer</t>
+  </si>
+  <si>
+    <t>Needs volume attention with mixer</t>
+  </si>
+  <si>
+    <t>Hellhound Ambiance</t>
+  </si>
+  <si>
+    <t>Vampire Ambiance</t>
+  </si>
+  <si>
+    <t>VampireAmbiance</t>
+  </si>
+  <si>
+    <t>HellhoundAmbiance</t>
+  </si>
+  <si>
+    <t>Having trouble because it doesn't recognize that there is a parameter</t>
   </si>
 </sst>
 </file>
@@ -708,10 +711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,16 +742,16 @@
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -756,7 +759,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
@@ -765,36 +768,36 @@
         <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
         <v>55</v>
-      </c>
-      <c r="B3" t="s">
-        <v>56</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -802,25 +805,25 @@
         <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -828,36 +831,36 @@
         <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>21</v>
@@ -869,30 +872,30 @@
         <v>21</v>
       </c>
       <c r="H6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" t="s">
         <v>60</v>
-      </c>
-      <c r="B7" t="s">
-        <v>61</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -900,22 +903,22 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -923,7 +926,7 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
         <v>16</v>
@@ -932,13 +935,13 @@
         <v>26</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -946,7 +949,7 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
         <v>16</v>
@@ -955,13 +958,13 @@
         <v>27</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -969,7 +972,7 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
         <v>15</v>
@@ -978,16 +981,16 @@
         <v>28</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -995,7 +998,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
         <v>15</v>
@@ -1004,16 +1007,16 @@
         <v>29</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1021,7 +1024,7 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
         <v>17</v>
@@ -1030,16 +1033,16 @@
         <v>30</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>21</v>
+        <v>71</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="H13" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1047,7 +1050,7 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
@@ -1056,13 +1059,13 @@
         <v>31</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1070,7 +1073,7 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
@@ -1079,62 +1082,62 @@
         <v>32</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1142,7 +1145,7 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
@@ -1151,13 +1154,13 @@
         <v>33</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>21</v>
+        <v>71</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1165,7 +1168,7 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
         <v>18</v>
@@ -1174,13 +1177,13 @@
         <v>34</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>21</v>
+        <v>71</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1188,7 +1191,7 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
         <v>18</v>
@@ -1197,143 +1200,169 @@
         <v>35</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>21</v>
+        <v>71</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
         <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>64</v>
+        <v>92</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H21" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>94</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C22" t="s">
         <v>15</v>
       </c>
       <c r="D22" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H22" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C23" t="s">
         <v>15</v>
       </c>
       <c r="D23" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="H23" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="C24" t="s">
         <v>15</v>
       </c>
       <c r="D24" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>21</v>
+        <v>71</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="H24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" t="s">
+        <v>87</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H26" t="s">
         <v>90</v>
-      </c>
-      <c r="B25" t="s">
-        <v>91</v>
-      </c>
-      <c r="C25" t="s">
-        <v>19</v>
-      </c>
-      <c r="D25" t="s">
-        <v>92</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H25" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added player health as a global parameter and also changed pitch of tutorial dialogue.
</commit_message>
<xml_diff>
--- a/documentation/AssetList.xlsx
+++ b/documentation/AssetList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\InteractiveGamesAndAudio\igme-671-final-project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7502C0-C668-4161-AFF3-B6D15F0C6DBB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997357D1-F30F-44FD-A229-C54C7DDEDB14}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="98">
   <si>
     <t>Description</t>
   </si>
@@ -291,9 +291,6 @@
     <t>Fire Crackling</t>
   </si>
   <si>
-    <t>May need to re-record with stereo eventually. Didn't realize it was only recording mono till it was already in FMOD and I'm not sure how much I like it</t>
-  </si>
-  <si>
     <t>Is playing, but volume needs some attention in mixer</t>
   </si>
   <si>
@@ -312,7 +309,16 @@
     <t>HellhoundAmbiance</t>
   </si>
   <si>
-    <t>Having trouble because it doesn't recognize that there is a parameter</t>
+    <t>Going to figure out how to pause</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fixed the one channel issue. My fault because of a setting I did with ReaEQ. I'm still not sure how much I like the sound though. </t>
+  </si>
+  <si>
+    <t>Maybe add enemy health paramater to enemy ambiance with spawn rates of scatterers</t>
+  </si>
+  <si>
+    <t>Player Health parameter is added. Will probably need some tweaking yet</t>
   </si>
 </sst>
 </file>
@@ -711,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1042,7 +1048,7 @@
         <v>71</v>
       </c>
       <c r="H13" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1162,6 +1168,9 @@
       <c r="G18" s="2" t="s">
         <v>71</v>
       </c>
+      <c r="H18" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -1185,6 +1194,9 @@
       <c r="G19" s="2" t="s">
         <v>71</v>
       </c>
+      <c r="H19" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -1211,7 +1223,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B21" t="s">
         <v>52</v>
@@ -1220,7 +1232,7 @@
         <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>71</v>
@@ -1228,16 +1240,13 @@
       <c r="F21" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H21" t="s">
-        <v>95</v>
+      <c r="G21" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B22" t="s">
         <v>52</v>
@@ -1246,7 +1255,7 @@
         <v>15</v>
       </c>
       <c r="D22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>71</v>
@@ -1254,11 +1263,8 @@
       <c r="F22" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H22" t="s">
-        <v>95</v>
+      <c r="G22" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1280,11 +1286,8 @@
       <c r="F23" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H23" t="s">
-        <v>95</v>
+      <c r="G23" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1336,7 +1339,7 @@
         <v>71</v>
       </c>
       <c r="H25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1362,7 +1365,17 @@
         <v>71</v>
       </c>
       <c r="H26" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H29" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Assets, implementation, and mixing should be done pending further comments.
</commit_message>
<xml_diff>
--- a/documentation/AssetList.xlsx
+++ b/documentation/AssetList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\InteractiveGamesAndAudio\igme-671-final-project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997357D1-F30F-44FD-A229-C54C7DDEDB14}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F33EA4E-40E3-4C5E-B6DC-2464F61A4252}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="94">
   <si>
     <t>Description</t>
   </si>
@@ -291,12 +291,6 @@
     <t>Fire Crackling</t>
   </si>
   <si>
-    <t>Is playing, but volume needs some attention in mixer</t>
-  </si>
-  <si>
-    <t>Needs volume attention with mixer</t>
-  </si>
-  <si>
     <t>Hellhound Ambiance</t>
   </si>
   <si>
@@ -307,12 +301,6 @@
   </si>
   <si>
     <t>HellhoundAmbiance</t>
-  </si>
-  <si>
-    <t>Going to figure out how to pause</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fixed the one channel issue. My fault because of a setting I did with ReaEQ. I'm still not sure how much I like the sound though. </t>
   </si>
   <si>
     <t>Maybe add enemy health paramater to enemy ambiance with spawn rates of scatterers</t>
@@ -720,7 +708,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,9 +1035,6 @@
       <c r="G13" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="H13" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1169,7 +1154,7 @@
         <v>71</v>
       </c>
       <c r="H18" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1195,7 +1180,7 @@
         <v>71</v>
       </c>
       <c r="H19" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1223,7 +1208,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B21" t="s">
         <v>52</v>
@@ -1232,7 +1217,7 @@
         <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>71</v>
@@ -1246,7 +1231,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B22" t="s">
         <v>52</v>
@@ -1255,7 +1240,7 @@
         <v>15</v>
       </c>
       <c r="D22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>71</v>
@@ -1338,9 +1323,6 @@
       <c r="G25" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="H25" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -1364,18 +1346,10 @@
       <c r="G26" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="H26" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H28" t="s">
-        <v>94</v>
-      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H29" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Should be finished with preliminary mixing and mastering.
</commit_message>
<xml_diff>
--- a/documentation/AssetList.xlsx
+++ b/documentation/AssetList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\InteractiveGamesAndAudio\igme-671-final-project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F33EA4E-40E3-4C5E-B6DC-2464F61A4252}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF376747-4C36-432C-96DB-F7CBAF46ED98}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -303,10 +303,10 @@
     <t>HellhoundAmbiance</t>
   </si>
   <si>
-    <t>Maybe add enemy health paramater to enemy ambiance with spawn rates of scatterers</t>
-  </si>
-  <si>
     <t>Player Health parameter is added. Will probably need some tweaking yet</t>
+  </si>
+  <si>
+    <t>Added enemy health as a parameter used with scaterrer event spawn rates and pitch</t>
   </si>
 </sst>
 </file>
@@ -708,7 +708,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1154,7 +1154,7 @@
         <v>71</v>
       </c>
       <c r="H18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1180,7 +1180,7 @@
         <v>71</v>
       </c>
       <c r="H19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1349,7 +1349,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H29" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Almost done incorporating feedback from Milestone 4. Still need to look at boss sounds and remix and master with consideration of other games.
</commit_message>
<xml_diff>
--- a/documentation/AssetList.xlsx
+++ b/documentation/AssetList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\InteractiveGamesAndAudio\igme-671-final-project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF376747-4C36-432C-96DB-F7CBAF46ED98}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C41DAE3-C3C2-4B83-901B-DF8A3D328B44}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="92">
   <si>
     <t>Description</t>
   </si>
@@ -219,15 +219,6 @@
     <t>Player Hit</t>
   </si>
   <si>
-    <t>PlayerDeath</t>
-  </si>
-  <si>
-    <t>An event indicating that the player has died</t>
-  </si>
-  <si>
-    <t>Player Death</t>
-  </si>
-  <si>
     <t>Vampire Hit, Hellhound Hit</t>
   </si>
   <si>
@@ -270,18 +261,9 @@
     <t>Ideally, won't shoot fireball as well, but that may be a code issue</t>
   </si>
   <si>
-    <t xml:space="preserve">Changed to 3D event. </t>
-  </si>
-  <si>
     <t>Not sure I like the vampire attack sound.</t>
   </si>
   <si>
-    <t xml:space="preserve">Not sure what sound I want to do for this exactly yet. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Changed to 3D event. Currently always playing if there is a healing tile in the level, but I'm not sure why. </t>
-  </si>
-  <si>
     <t>Staff Fire Crackling</t>
   </si>
   <si>
@@ -303,10 +285,22 @@
     <t>HellhoundAmbiance</t>
   </si>
   <si>
-    <t>Player Health parameter is added. Will probably need some tweaking yet</t>
-  </si>
-  <si>
-    <t>Added enemy health as a parameter used with scaterrer event spawn rates and pitch</t>
+    <t>Mouseover</t>
+  </si>
+  <si>
+    <t>A sound to indicate the mouse going over a button</t>
+  </si>
+  <si>
+    <t>Player Health Alert</t>
+  </si>
+  <si>
+    <t>A sound to add in when the player's health is low</t>
+  </si>
+  <si>
+    <t>Alert Sound</t>
+  </si>
+  <si>
+    <t>Vampire Boss</t>
   </si>
 </sst>
 </file>
@@ -705,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,16 +730,16 @@
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -762,13 +756,13 @@
         <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -782,16 +776,16 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -808,16 +802,16 @@
         <v>62</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -834,381 +828,366 @@
         <v>63</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" t="s">
-        <v>83</v>
+        <v>61</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
         <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
         <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H11" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H12" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="H16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H18" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H19" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B21" t="s">
         <v>52</v>
@@ -1217,139 +1196,168 @@
         <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>91</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
         <v>15</v>
       </c>
       <c r="D22" t="s">
-        <v>88</v>
+        <v>36</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C23" t="s">
         <v>15</v>
       </c>
       <c r="D23" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="C24" t="s">
         <v>15</v>
       </c>
       <c r="D24" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H24" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B25" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C25" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D25" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B26" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C26" t="s">
         <v>19</v>
       </c>
       <c r="D26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H29" t="s">
-        <v>93</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>91</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finishing up tweaks for Final Submission.
</commit_message>
<xml_diff>
--- a/documentation/AssetList.xlsx
+++ b/documentation/AssetList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\InteractiveGamesAndAudio\igme-671-final-project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C41DAE3-C3C2-4B83-901B-DF8A3D328B44}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32818B91-7B38-49A1-A3AE-A8B0D9A44949}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="97">
   <si>
     <t>Description</t>
   </si>
@@ -90,9 +90,6 @@
     <t>PlayerAmbiance</t>
   </si>
   <si>
-    <t>Incomplete</t>
-  </si>
-  <si>
     <t>Fireball Fire, Fireball Charge</t>
   </si>
   <si>
@@ -300,7 +297,25 @@
     <t>Alert Sound</t>
   </si>
   <si>
-    <t>Vampire Boss</t>
+    <t>Stone Door Opening</t>
+  </si>
+  <si>
+    <t>Boss Death</t>
+  </si>
+  <si>
+    <t>Hellhound Death</t>
+  </si>
+  <si>
+    <t>Vampire Boss Death</t>
+  </si>
+  <si>
+    <t>A sound to indicate that the boss has died</t>
+  </si>
+  <si>
+    <t>A sound to indicate that a hellhound has died</t>
+  </si>
+  <si>
+    <t>A sound to indicate that a stone door that was previously closed has opened</t>
   </si>
 </sst>
 </file>
@@ -332,7 +347,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -342,12 +357,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -409,10 +418,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -699,10 +707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,29 +725,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="H1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>70</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -747,140 +755,140 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>68</v>
+        <v>21</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
         <v>54</v>
-      </c>
-      <c r="B3" t="s">
-        <v>55</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>68</v>
+        <v>61</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="H4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>68</v>
+        <v>62</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" t="s">
         <v>59</v>
-      </c>
-      <c r="B6" t="s">
-        <v>60</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -888,22 +896,22 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>68</v>
+        <v>25</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -911,22 +919,22 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
         <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>68</v>
+        <v>26</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -934,22 +942,22 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>68</v>
+        <v>27</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -957,22 +965,22 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
         <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>68</v>
+        <v>28</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -980,22 +988,22 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>68</v>
+        <v>29</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1003,22 +1011,22 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
         <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>68</v>
+        <v>30</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1026,71 +1034,71 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>68</v>
+        <v>31</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" t="s">
         <v>73</v>
-      </c>
-      <c r="B15" t="s">
-        <v>74</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>68</v>
+      <c r="E16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="H16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1098,22 +1106,22 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
         <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>68</v>
+        <v>32</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1121,22 +1129,22 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>68</v>
+        <v>33</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1144,68 +1152,68 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>68</v>
+        <v>34</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
         <v>15</v>
       </c>
       <c r="D20" t="s">
-        <v>83</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>68</v>
+        <v>82</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
         <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>82</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>68</v>
+        <v>81</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1213,151 +1221,206 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C22" t="s">
         <v>15</v>
       </c>
       <c r="D22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>68</v>
+        <v>35</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" t="s">
         <v>56</v>
-      </c>
-      <c r="B23" t="s">
-        <v>57</v>
       </c>
       <c r="C23" t="s">
         <v>15</v>
       </c>
       <c r="D23" t="s">
-        <v>58</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>68</v>
+        <v>57</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" t="s">
         <v>75</v>
-      </c>
-      <c r="B24" t="s">
-        <v>76</v>
       </c>
       <c r="C24" t="s">
         <v>15</v>
       </c>
       <c r="D24" t="s">
-        <v>75</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" t="s">
         <v>79</v>
-      </c>
-      <c r="B25" t="s">
-        <v>80</v>
       </c>
       <c r="C25" t="s">
         <v>19</v>
       </c>
       <c r="D25" t="s">
-        <v>81</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>68</v>
+        <v>80</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" t="s">
         <v>86</v>
-      </c>
-      <c r="B26" t="s">
-        <v>87</v>
       </c>
       <c r="C26" t="s">
         <v>19</v>
       </c>
       <c r="D26" t="s">
-        <v>86</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>68</v>
+        <v>85</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27" t="s">
         <v>88</v>
-      </c>
-      <c r="B27" t="s">
-        <v>89</v>
       </c>
       <c r="C27" t="s">
         <v>15</v>
       </c>
       <c r="D27" t="s">
-        <v>90</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>68</v>
+        <v>89</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" t="s">
         <v>91</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>21</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" t="s">
+        <v>92</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" t="s">
+        <v>90</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>